<commit_message>
added to 2010 election results
</commit_message>
<xml_diff>
--- a/2010_Election_Results_TNT_clean.xlsx
+++ b/2010_Election_Results_TNT_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosspingatore/Desktop/Practicum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharyl/Desktop/Other/proj/Inclusion_by_Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481C9611-E5A6-B141-BA73-8B2A9F3DAE17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0247F4C3-C37A-E940-9B54-C1AB00273525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38460" yWindow="500" windowWidth="38400" windowHeight="21800" xr2:uid="{92ED79AB-027C-6E40-8484-828CF8073DBC}"/>
+    <workbookView xWindow="-5280" yWindow="0" windowWidth="18500" windowHeight="16000" xr2:uid="{92ED79AB-027C-6E40-8484-828CF8073DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="2010_Election_Results_TNT" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2845" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2949" uniqueCount="803">
   <si>
     <t>Electoral_Dist</t>
   </si>
@@ -2321,6 +2321,129 @@
   </si>
   <si>
     <t xml:space="preserve">BICHE </t>
+  </si>
+  <si>
+    <t>D'Abadie/O'Meara</t>
+  </si>
+  <si>
+    <t>1806_02</t>
+  </si>
+  <si>
+    <t>Pine Ha en S.D.A Primary School</t>
+  </si>
+  <si>
+    <t>LP #18 LA Resource Road South</t>
+  </si>
+  <si>
+    <t>D'Abadie</t>
+  </si>
+  <si>
+    <t>1806_03</t>
+  </si>
+  <si>
+    <t>1806_04</t>
+  </si>
+  <si>
+    <t>1950_01</t>
+  </si>
+  <si>
+    <t>1950_02</t>
+  </si>
+  <si>
+    <t>1955_01</t>
+  </si>
+  <si>
+    <t>1955_02</t>
+  </si>
+  <si>
+    <t>D'Abadie Government Primary School</t>
+  </si>
+  <si>
+    <t>LP 557 Eastern Main Road</t>
+  </si>
+  <si>
+    <t>1955_03</t>
+  </si>
+  <si>
+    <t>1955_04</t>
+  </si>
+  <si>
+    <t>1960_01</t>
+  </si>
+  <si>
+    <t>1960_02</t>
+  </si>
+  <si>
+    <t>1960_03</t>
+  </si>
+  <si>
+    <t>1961_01</t>
+  </si>
+  <si>
+    <t>1961_02</t>
+  </si>
+  <si>
+    <t>Ministry of Works and Transport</t>
+  </si>
+  <si>
+    <t>St. George East, O'Meara Road</t>
+  </si>
+  <si>
+    <t>1965_01</t>
+  </si>
+  <si>
+    <t>1965_02</t>
+  </si>
+  <si>
+    <t>1966_01</t>
+  </si>
+  <si>
+    <t>1966_02</t>
+  </si>
+  <si>
+    <t>*1967</t>
+  </si>
+  <si>
+    <t>1969_1</t>
+  </si>
+  <si>
+    <t>Malabar Government Primary School</t>
+  </si>
+  <si>
+    <t>Arima Presbytarian Primary School</t>
+  </si>
+  <si>
+    <t>Larry Gomes Stadium</t>
+  </si>
+  <si>
+    <t>Malabar Secondary School</t>
+  </si>
+  <si>
+    <t>Pomegranate Avenue, Phase 1</t>
+  </si>
+  <si>
+    <t>Pomegranate Avenue, Phase 2</t>
+  </si>
+  <si>
+    <t>Tupuna Road</t>
+  </si>
+  <si>
+    <t>Nutones Bouleard</t>
+  </si>
+  <si>
+    <t>Flamingo Boulevard, Phase 4, Section 2</t>
+  </si>
+  <si>
+    <t>Flamingo Boulevard, Phase 4, Section 3</t>
+  </si>
+  <si>
+    <t>Malabar, Arima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malabar </t>
+  </si>
+  <si>
+    <t>Malabar</t>
   </si>
 </sst>
 </file>
@@ -2749,11 +2872,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF65B61F-06D8-774A-83EF-A02372F67DE5}">
-  <dimension ref="A1:P510"/>
+  <dimension ref="A1:P533"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E529" sqref="E529"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A507" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P534" sqref="P534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27524,6 +27647,1018 @@
         <v>395</v>
       </c>
     </row>
+    <row r="511" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A511" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B511" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C511" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="D511" t="s">
+        <v>764</v>
+      </c>
+      <c r="E511" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="F511" t="s">
+        <v>766</v>
+      </c>
+      <c r="H511">
+        <v>282</v>
+      </c>
+      <c r="I511" s="12">
+        <v>0</v>
+      </c>
+      <c r="J511">
+        <v>237</v>
+      </c>
+      <c r="K511">
+        <v>0</v>
+      </c>
+      <c r="L511">
+        <v>0</v>
+      </c>
+      <c r="M511">
+        <v>0</v>
+      </c>
+      <c r="N511">
+        <v>4</v>
+      </c>
+      <c r="O511">
+        <v>523</v>
+      </c>
+      <c r="P511" s="14">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="512" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A512" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B512" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C512" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="D512" t="s">
+        <v>764</v>
+      </c>
+      <c r="E512" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="F512" t="s">
+        <v>766</v>
+      </c>
+      <c r="H512">
+        <v>256</v>
+      </c>
+      <c r="I512" s="12">
+        <v>0</v>
+      </c>
+      <c r="J512">
+        <v>216</v>
+      </c>
+      <c r="K512">
+        <v>0</v>
+      </c>
+      <c r="L512">
+        <v>0</v>
+      </c>
+      <c r="M512">
+        <v>0</v>
+      </c>
+      <c r="N512">
+        <v>1</v>
+      </c>
+      <c r="O512">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="513" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A513" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B513" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D513" t="s">
+        <v>764</v>
+      </c>
+      <c r="E513" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="F513" t="s">
+        <v>766</v>
+      </c>
+      <c r="H513">
+        <v>221</v>
+      </c>
+      <c r="I513" s="12">
+        <v>0</v>
+      </c>
+      <c r="J513">
+        <v>252</v>
+      </c>
+      <c r="K513">
+        <v>0</v>
+      </c>
+      <c r="L513">
+        <v>0</v>
+      </c>
+      <c r="M513">
+        <v>0</v>
+      </c>
+      <c r="N513">
+        <v>1</v>
+      </c>
+      <c r="O513">
+        <v>474</v>
+      </c>
+      <c r="P513" s="14">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="514" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A514" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B514" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C514" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D514" t="s">
+        <v>25</v>
+      </c>
+      <c r="E514" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F514" t="s">
+        <v>766</v>
+      </c>
+      <c r="H514">
+        <v>263</v>
+      </c>
+      <c r="I514" s="12">
+        <v>0</v>
+      </c>
+      <c r="J514">
+        <v>201</v>
+      </c>
+      <c r="K514">
+        <v>0</v>
+      </c>
+      <c r="L514">
+        <v>0</v>
+      </c>
+      <c r="M514">
+        <v>0</v>
+      </c>
+      <c r="N514">
+        <v>3</v>
+      </c>
+      <c r="O514">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="515" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A515" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B515" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C515" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="D515" t="s">
+        <v>25</v>
+      </c>
+      <c r="E515" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F515" t="s">
+        <v>766</v>
+      </c>
+      <c r="H515">
+        <v>205</v>
+      </c>
+      <c r="I515" s="12">
+        <v>0</v>
+      </c>
+      <c r="J515">
+        <v>209</v>
+      </c>
+      <c r="K515">
+        <v>0</v>
+      </c>
+      <c r="L515">
+        <v>0</v>
+      </c>
+      <c r="M515">
+        <v>0</v>
+      </c>
+      <c r="N515">
+        <v>0</v>
+      </c>
+      <c r="O515">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="516" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A516" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B516" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C516" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="D516" t="s">
+        <v>773</v>
+      </c>
+      <c r="E516" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="F516" t="s">
+        <v>766</v>
+      </c>
+      <c r="H516">
+        <v>216</v>
+      </c>
+      <c r="I516" s="12">
+        <v>0</v>
+      </c>
+      <c r="J516">
+        <v>261</v>
+      </c>
+      <c r="K516">
+        <v>0</v>
+      </c>
+      <c r="L516">
+        <v>0</v>
+      </c>
+      <c r="M516">
+        <v>0</v>
+      </c>
+      <c r="N516">
+        <v>6</v>
+      </c>
+      <c r="O516">
+        <v>483</v>
+      </c>
+      <c r="P516" s="14">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="517" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A517" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B517" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="D517" t="s">
+        <v>773</v>
+      </c>
+      <c r="E517" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="F517" t="s">
+        <v>766</v>
+      </c>
+      <c r="H517">
+        <v>242</v>
+      </c>
+      <c r="I517" s="12">
+        <v>0</v>
+      </c>
+      <c r="J517">
+        <v>184</v>
+      </c>
+      <c r="K517">
+        <v>0</v>
+      </c>
+      <c r="L517">
+        <v>0</v>
+      </c>
+      <c r="M517">
+        <v>0</v>
+      </c>
+      <c r="N517">
+        <v>0</v>
+      </c>
+      <c r="O517">
+        <v>426</v>
+      </c>
+      <c r="P517" s="14">
+        <v>6108</v>
+      </c>
+    </row>
+    <row r="518" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A518" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B518" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C518" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="D518" t="s">
+        <v>773</v>
+      </c>
+      <c r="E518" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="F518" t="s">
+        <v>766</v>
+      </c>
+      <c r="H518">
+        <v>1685</v>
+      </c>
+      <c r="I518" s="12">
+        <v>0</v>
+      </c>
+      <c r="J518">
+        <v>1560</v>
+      </c>
+      <c r="K518">
+        <v>0</v>
+      </c>
+      <c r="L518">
+        <v>0</v>
+      </c>
+      <c r="M518">
+        <v>0</v>
+      </c>
+      <c r="N518">
+        <v>15</v>
+      </c>
+      <c r="O518">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="519" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A519" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B519" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C519" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="D519" t="s">
+        <v>773</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="F519" t="s">
+        <v>766</v>
+      </c>
+      <c r="H519">
+        <v>200</v>
+      </c>
+      <c r="I519" s="12">
+        <v>0</v>
+      </c>
+      <c r="J519">
+        <v>224</v>
+      </c>
+      <c r="K519">
+        <v>0</v>
+      </c>
+      <c r="L519">
+        <v>0</v>
+      </c>
+      <c r="M519">
+        <v>0</v>
+      </c>
+      <c r="N519">
+        <v>0</v>
+      </c>
+      <c r="O519">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="520" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A520" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B520" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C520" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="D520" t="s">
+        <v>782</v>
+      </c>
+      <c r="E520" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="F520" t="s">
+        <v>5</v>
+      </c>
+      <c r="H520">
+        <v>253</v>
+      </c>
+      <c r="I520" s="12">
+        <v>0</v>
+      </c>
+      <c r="J520">
+        <v>299</v>
+      </c>
+      <c r="K520">
+        <v>0</v>
+      </c>
+      <c r="L520">
+        <v>0</v>
+      </c>
+      <c r="M520">
+        <v>0</v>
+      </c>
+      <c r="N520">
+        <v>2</v>
+      </c>
+      <c r="O520">
+        <v>554</v>
+      </c>
+      <c r="P520" s="14">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="521" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A521" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B521" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C521" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="D521" t="s">
+        <v>782</v>
+      </c>
+      <c r="E521" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="F521" t="s">
+        <v>5</v>
+      </c>
+      <c r="H521">
+        <v>191</v>
+      </c>
+      <c r="I521" s="12">
+        <v>0</v>
+      </c>
+      <c r="J521">
+        <v>141</v>
+      </c>
+      <c r="K521">
+        <v>0</v>
+      </c>
+      <c r="L521">
+        <v>0</v>
+      </c>
+      <c r="M521">
+        <v>0</v>
+      </c>
+      <c r="N521">
+        <v>2</v>
+      </c>
+      <c r="O521">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="522" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A522" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B522" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C522" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="D522" t="s">
+        <v>782</v>
+      </c>
+      <c r="E522" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="F522" t="s">
+        <v>5</v>
+      </c>
+      <c r="H522">
+        <v>199</v>
+      </c>
+      <c r="I522" s="12">
+        <v>0</v>
+      </c>
+      <c r="J522">
+        <v>139</v>
+      </c>
+      <c r="K522">
+        <v>0</v>
+      </c>
+      <c r="L522">
+        <v>0</v>
+      </c>
+      <c r="M522">
+        <v>0</v>
+      </c>
+      <c r="N522">
+        <v>5</v>
+      </c>
+      <c r="O522">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="523" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A523" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B523" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C523" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D523" t="s">
+        <v>782</v>
+      </c>
+      <c r="E523" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="F523" t="s">
+        <v>5</v>
+      </c>
+      <c r="H523">
+        <v>188</v>
+      </c>
+      <c r="I523" s="12">
+        <v>0</v>
+      </c>
+      <c r="J523">
+        <v>218</v>
+      </c>
+      <c r="K523">
+        <v>0</v>
+      </c>
+      <c r="L523">
+        <v>0</v>
+      </c>
+      <c r="M523">
+        <v>0</v>
+      </c>
+      <c r="N523">
+        <v>4</v>
+      </c>
+      <c r="O523">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="524" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A524" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B524" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C524" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="D524" t="s">
+        <v>782</v>
+      </c>
+      <c r="E524" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="F524" t="s">
+        <v>5</v>
+      </c>
+      <c r="H524">
+        <v>122</v>
+      </c>
+      <c r="I524" s="12">
+        <v>0</v>
+      </c>
+      <c r="J524">
+        <v>218</v>
+      </c>
+      <c r="K524">
+        <v>0</v>
+      </c>
+      <c r="L524">
+        <v>0</v>
+      </c>
+      <c r="M524">
+        <v>0</v>
+      </c>
+      <c r="N524">
+        <v>0</v>
+      </c>
+      <c r="O524">
+        <v>340</v>
+      </c>
+      <c r="P524" s="14">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="525" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A525" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B525" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C525" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D525" t="s">
+        <v>790</v>
+      </c>
+      <c r="E525" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="F525" t="s">
+        <v>800</v>
+      </c>
+      <c r="H525">
+        <v>110</v>
+      </c>
+      <c r="I525" s="12">
+        <v>0</v>
+      </c>
+      <c r="J525">
+        <v>222</v>
+      </c>
+      <c r="K525">
+        <v>0</v>
+      </c>
+      <c r="L525">
+        <v>0</v>
+      </c>
+      <c r="M525">
+        <v>0</v>
+      </c>
+      <c r="N525">
+        <v>2</v>
+      </c>
+      <c r="O525">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="526" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A526" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B526" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C526" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="D526" t="s">
+        <v>790</v>
+      </c>
+      <c r="E526" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="F526" t="s">
+        <v>800</v>
+      </c>
+      <c r="H526">
+        <v>2948</v>
+      </c>
+      <c r="I526" s="12">
+        <v>0</v>
+      </c>
+      <c r="J526" s="12">
+        <v>3021</v>
+      </c>
+      <c r="K526">
+        <v>0</v>
+      </c>
+      <c r="L526">
+        <v>0</v>
+      </c>
+      <c r="M526">
+        <v>0</v>
+      </c>
+      <c r="N526">
+        <v>30</v>
+      </c>
+      <c r="O526">
+        <v>5999</v>
+      </c>
+      <c r="P526" s="14">
+        <v>8739</v>
+      </c>
+    </row>
+    <row r="527" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A527" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B527" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C527" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="D527" t="s">
+        <v>791</v>
+      </c>
+      <c r="E527" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="F527" t="s">
+        <v>5</v>
+      </c>
+      <c r="H527">
+        <v>172</v>
+      </c>
+      <c r="I527" s="12">
+        <v>0</v>
+      </c>
+      <c r="J527" s="12">
+        <v>55</v>
+      </c>
+      <c r="K527">
+        <v>0</v>
+      </c>
+      <c r="L527">
+        <v>0</v>
+      </c>
+      <c r="M527">
+        <v>0</v>
+      </c>
+      <c r="N527">
+        <v>1</v>
+      </c>
+      <c r="O527">
+        <v>228</v>
+      </c>
+      <c r="P527" s="14">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="528" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A528" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B528" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C528" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="D528" t="s">
+        <v>791</v>
+      </c>
+      <c r="E528" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="F528" t="s">
+        <v>5</v>
+      </c>
+      <c r="H528">
+        <v>175</v>
+      </c>
+      <c r="I528" s="12">
+        <v>0</v>
+      </c>
+      <c r="J528" s="12">
+        <v>97</v>
+      </c>
+      <c r="K528">
+        <v>0</v>
+      </c>
+      <c r="L528">
+        <v>0</v>
+      </c>
+      <c r="M528">
+        <v>0</v>
+      </c>
+      <c r="N528">
+        <v>0</v>
+      </c>
+      <c r="O528">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="529" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A529" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B529" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C529" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="D529" t="s">
+        <v>792</v>
+      </c>
+      <c r="E529" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="F529" t="s">
+        <v>800</v>
+      </c>
+      <c r="H529">
+        <v>132</v>
+      </c>
+      <c r="I529" s="12">
+        <v>0</v>
+      </c>
+      <c r="J529" s="12">
+        <v>165</v>
+      </c>
+      <c r="K529">
+        <v>0</v>
+      </c>
+      <c r="L529">
+        <v>0</v>
+      </c>
+      <c r="M529">
+        <v>0</v>
+      </c>
+      <c r="N529">
+        <v>1</v>
+      </c>
+      <c r="O529">
+        <v>298</v>
+      </c>
+      <c r="P529" s="14">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="530" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A530" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B530" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C530" s="2">
+        <v>1968</v>
+      </c>
+      <c r="D530" t="s">
+        <v>793</v>
+      </c>
+      <c r="E530" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="F530" t="s">
+        <v>801</v>
+      </c>
+      <c r="H530">
+        <v>100</v>
+      </c>
+      <c r="I530" s="12">
+        <v>0</v>
+      </c>
+      <c r="J530" s="12">
+        <v>199</v>
+      </c>
+      <c r="K530">
+        <v>0</v>
+      </c>
+      <c r="L530">
+        <v>0</v>
+      </c>
+      <c r="M530">
+        <v>0</v>
+      </c>
+      <c r="N530">
+        <v>0</v>
+      </c>
+      <c r="O530">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="531" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A531" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B531" s="12">
+        <v>2010</v>
+      </c>
+      <c r="C531" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="D531" t="s">
+        <v>793</v>
+      </c>
+      <c r="E531" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="F531" t="s">
+        <v>802</v>
+      </c>
+      <c r="H531">
+        <v>584</v>
+      </c>
+      <c r="I531" s="12">
+        <v>0</v>
+      </c>
+      <c r="J531" s="12">
+        <v>229</v>
+      </c>
+      <c r="K531">
+        <v>0</v>
+      </c>
+      <c r="L531">
+        <v>0</v>
+      </c>
+      <c r="M531">
+        <v>0</v>
+      </c>
+      <c r="N531">
+        <v>0</v>
+      </c>
+      <c r="O531">
+        <v>813</v>
+      </c>
+      <c r="P531" s="14">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="532" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H532">
+        <v>162</v>
+      </c>
+      <c r="I532" s="12">
+        <v>0</v>
+      </c>
+      <c r="J532" s="12">
+        <v>156</v>
+      </c>
+      <c r="K532">
+        <v>0</v>
+      </c>
+      <c r="L532">
+        <v>0</v>
+      </c>
+      <c r="M532">
+        <v>0</v>
+      </c>
+      <c r="N532">
+        <v>0</v>
+      </c>
+      <c r="O532">
+        <v>318</v>
+      </c>
+      <c r="P532" s="14">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="533" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H533">
+        <v>198</v>
+      </c>
+      <c r="I533" s="12">
+        <v>0</v>
+      </c>
+      <c r="J533" s="12">
+        <v>118</v>
+      </c>
+      <c r="K533">
+        <v>0</v>
+      </c>
+      <c r="L533">
+        <v>0</v>
+      </c>
+      <c r="M533">
+        <v>0</v>
+      </c>
+      <c r="N533">
+        <v>0</v>
+      </c>
+      <c r="O533">
+        <v>316</v>
+      </c>
+      <c r="P533" s="14">
+        <v>899</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>